<commit_message>
Added neighborhood, fixed helper functions, replaced sspace with solutionMatrices
</commit_message>
<xml_diff>
--- a/steady.xlsx
+++ b/steady.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="1505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="1859">
   <si>
     <t>Row</t>
   </si>
@@ -1339,6 +1339,1068 @@
   </si>
   <si>
     <t>Autoregression in 5-year term premium</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Infl</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Wage</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>dA</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R20exp</t>
+  </si>
+  <si>
+    <t>term20</t>
+  </si>
+  <si>
+    <t>Pk</t>
+  </si>
+  <si>
+    <t>Rk</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>dP</t>
+  </si>
+  <si>
+    <t>d4P</t>
+  </si>
+  <si>
+    <t>dW</t>
+  </si>
+  <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>Mp</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>Ey</t>
+  </si>
+  <si>
+    <t>Ep</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t>Er</t>
+  </si>
+  <si>
+    <t>Eterm20</t>
+  </si>
+  <si>
+    <t>Ew</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>xiw</t>
+  </si>
+  <si>
+    <t>xip</t>
+  </si>
+  <si>
+    <t>rhoa</t>
+  </si>
+  <si>
+    <t>rhor</t>
+  </si>
+  <si>
+    <t>kappap</t>
+  </si>
+  <si>
+    <t>kappan</t>
+  </si>
+  <si>
+    <t>rhoterm20</t>
+  </si>
+  <si>
+    <t>Short_</t>
+  </si>
+  <si>
+    <t>Long_</t>
+  </si>
+  <si>
+    <t>Infl_</t>
+  </si>
+  <si>
+    <t>Growth_</t>
+  </si>
+  <si>
+    <t>Wage_</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Short term rate</t>
+  </si>
+  <si>
+    <t>Long term rate</t>
+  </si>
+  <si>
+    <t>Price inflation</t>
+  </si>
+  <si>
+    <t>Output growth</t>
+  </si>
+  <si>
+    <t>Wage inflation</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Wage rate</t>
+  </si>
+  <si>
+    <t>Nominal marginal cost</t>
+  </si>
+  <si>
+    <t>Consumption habit</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Rate of change in productivity</t>
+  </si>
+  <si>
+    <t>Final prices</t>
+  </si>
+  <si>
+    <t>Interest rate</t>
+  </si>
+  <si>
+    <t>5-year interest rate</t>
+  </si>
+  <si>
+    <t>5-Year expectations of short rates</t>
+  </si>
+  <si>
+    <t>5-year term premium</t>
+  </si>
+  <si>
+    <t>Price of capital</t>
+  </si>
+  <si>
+    <t>Rental price of capital</t>
+  </si>
+  <si>
+    <t>Households shadow value of wealth</t>
+  </si>
+  <si>
+    <t>Inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Inflation Y/Y</t>
+  </si>
+  <si>
+    <t>Wage inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Real marginal cost</t>
+  </si>
+  <si>
+    <t>Measurement error on price inflation</t>
+  </si>
+  <si>
+    <t>Measurement error on wage inflation</t>
+  </si>
+  <si>
+    <t>Consumption demand shock</t>
+  </si>
+  <si>
+    <t>Cost push shock</t>
+  </si>
+  <si>
+    <t>Productivity shock</t>
+  </si>
+  <si>
+    <t>Policy shock</t>
+  </si>
+  <si>
+    <t>Long-term rate shock</t>
+  </si>
+  <si>
+    <t>Wage shock</t>
+  </si>
+  <si>
+    <t>Long run growth</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Labor share</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Fixed level of capital</t>
+  </si>
+  <si>
+    <t>Inflation target</t>
+  </si>
+  <si>
+    <t>Elasticity of substitution in monopoly markets</t>
+  </si>
+  <si>
+    <t>Inverse elasticity of labor supply</t>
+  </si>
+  <si>
+    <t>Habit</t>
+  </si>
+  <si>
+    <t>Wage stickiness</t>
+  </si>
+  <si>
+    <t>Price stickiness</t>
+  </si>
+  <si>
+    <t>Autoregression in productivity</t>
+  </si>
+  <si>
+    <t>Autoregression in short rate</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to inflation</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to labor</t>
+  </si>
+  <si>
+    <t>Autoregression in 5-year term premium</t>
+  </si>
+  <si>
+    <t>Intercept in short rate</t>
+  </si>
+  <si>
+    <t>Intercept in long rate</t>
+  </si>
+  <si>
+    <t>Intercept in inflation rate</t>
+  </si>
+  <si>
+    <t>Intercept in output growth rate</t>
+  </si>
+  <si>
+    <t>Intercept in wage inflation rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Infl</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Wage</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>dA</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R20exp</t>
+  </si>
+  <si>
+    <t>term20</t>
+  </si>
+  <si>
+    <t>Pk</t>
+  </si>
+  <si>
+    <t>Rk</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>dP</t>
+  </si>
+  <si>
+    <t>d4P</t>
+  </si>
+  <si>
+    <t>dW</t>
+  </si>
+  <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>Mp</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>Ey</t>
+  </si>
+  <si>
+    <t>Ep</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t>Er</t>
+  </si>
+  <si>
+    <t>Eterm20</t>
+  </si>
+  <si>
+    <t>Ew</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>xiw</t>
+  </si>
+  <si>
+    <t>xip</t>
+  </si>
+  <si>
+    <t>rhoa</t>
+  </si>
+  <si>
+    <t>rhor</t>
+  </si>
+  <si>
+    <t>kappap</t>
+  </si>
+  <si>
+    <t>kappan</t>
+  </si>
+  <si>
+    <t>rhoterm20</t>
+  </si>
+  <si>
+    <t>Short_</t>
+  </si>
+  <si>
+    <t>Long_</t>
+  </si>
+  <si>
+    <t>Infl_</t>
+  </si>
+  <si>
+    <t>Growth_</t>
+  </si>
+  <si>
+    <t>Wage_</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Short term rate</t>
+  </si>
+  <si>
+    <t>Long term rate</t>
+  </si>
+  <si>
+    <t>Price inflation</t>
+  </si>
+  <si>
+    <t>Output growth</t>
+  </si>
+  <si>
+    <t>Wage inflation</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Wage rate</t>
+  </si>
+  <si>
+    <t>Nominal marginal cost</t>
+  </si>
+  <si>
+    <t>Consumption habit</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Rate of change in productivity</t>
+  </si>
+  <si>
+    <t>Final prices</t>
+  </si>
+  <si>
+    <t>Interest rate</t>
+  </si>
+  <si>
+    <t>5-year interest rate</t>
+  </si>
+  <si>
+    <t>5-Year expectations of short rates</t>
+  </si>
+  <si>
+    <t>5-year term premium</t>
+  </si>
+  <si>
+    <t>Price of capital</t>
+  </si>
+  <si>
+    <t>Rental price of capital</t>
+  </si>
+  <si>
+    <t>Households shadow value of wealth</t>
+  </si>
+  <si>
+    <t>Inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Inflation Y/Y</t>
+  </si>
+  <si>
+    <t>Wage inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Real marginal cost</t>
+  </si>
+  <si>
+    <t>Measurement error on price inflation</t>
+  </si>
+  <si>
+    <t>Measurement error on wage inflation</t>
+  </si>
+  <si>
+    <t>Consumption demand shock</t>
+  </si>
+  <si>
+    <t>Cost push shock</t>
+  </si>
+  <si>
+    <t>Productivity shock</t>
+  </si>
+  <si>
+    <t>Policy shock</t>
+  </si>
+  <si>
+    <t>Long-term rate shock</t>
+  </si>
+  <si>
+    <t>Wage shock</t>
+  </si>
+  <si>
+    <t>Long run growth</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Labor share</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Fixed level of capital</t>
+  </si>
+  <si>
+    <t>Inflation target</t>
+  </si>
+  <si>
+    <t>Elasticity of substitution in monopoly markets</t>
+  </si>
+  <si>
+    <t>Inverse elasticity of labor supply</t>
+  </si>
+  <si>
+    <t>Habit</t>
+  </si>
+  <si>
+    <t>Wage stickiness</t>
+  </si>
+  <si>
+    <t>Price stickiness</t>
+  </si>
+  <si>
+    <t>Autoregression in productivity</t>
+  </si>
+  <si>
+    <t>Autoregression in short rate</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to inflation</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to labor</t>
+  </si>
+  <si>
+    <t>Autoregression in 5-year term premium</t>
+  </si>
+  <si>
+    <t>Intercept in short rate</t>
+  </si>
+  <si>
+    <t>Intercept in long rate</t>
+  </si>
+  <si>
+    <t>Intercept in inflation rate</t>
+  </si>
+  <si>
+    <t>Intercept in output growth rate</t>
+  </si>
+  <si>
+    <t>Intercept in wage inflation rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Infl</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Wage</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>dA</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R20exp</t>
+  </si>
+  <si>
+    <t>term20</t>
+  </si>
+  <si>
+    <t>Pk</t>
+  </si>
+  <si>
+    <t>Rk</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>dP</t>
+  </si>
+  <si>
+    <t>d4P</t>
+  </si>
+  <si>
+    <t>dW</t>
+  </si>
+  <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>Mp</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>Ey</t>
+  </si>
+  <si>
+    <t>Ep</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t>Er</t>
+  </si>
+  <si>
+    <t>Eterm20</t>
+  </si>
+  <si>
+    <t>Ew</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>xiw</t>
+  </si>
+  <si>
+    <t>xip</t>
+  </si>
+  <si>
+    <t>rhoa</t>
+  </si>
+  <si>
+    <t>rhor</t>
+  </si>
+  <si>
+    <t>kappap</t>
+  </si>
+  <si>
+    <t>kappan</t>
+  </si>
+  <si>
+    <t>rhoterm20</t>
+  </si>
+  <si>
+    <t>Short_</t>
+  </si>
+  <si>
+    <t>Long_</t>
+  </si>
+  <si>
+    <t>Infl_</t>
+  </si>
+  <si>
+    <t>Growth_</t>
+  </si>
+  <si>
+    <t>Wage_</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel</t>
+  </si>
+  <si>
+    <t>SteadyChange</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Short term rate</t>
+  </si>
+  <si>
+    <t>Long term rate</t>
+  </si>
+  <si>
+    <t>Price inflation</t>
+  </si>
+  <si>
+    <t>Output growth</t>
+  </si>
+  <si>
+    <t>Wage inflation</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Wage rate</t>
+  </si>
+  <si>
+    <t>Nominal marginal cost</t>
+  </si>
+  <si>
+    <t>Consumption habit</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Rate of change in productivity</t>
+  </si>
+  <si>
+    <t>Final prices</t>
+  </si>
+  <si>
+    <t>Interest rate</t>
+  </si>
+  <si>
+    <t>5-year interest rate</t>
+  </si>
+  <si>
+    <t>5-Year expectations of short rates</t>
+  </si>
+  <si>
+    <t>5-year term premium</t>
+  </si>
+  <si>
+    <t>Price of capital</t>
+  </si>
+  <si>
+    <t>Rental price of capital</t>
+  </si>
+  <si>
+    <t>Households shadow value of wealth</t>
+  </si>
+  <si>
+    <t>Inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Inflation Y/Y</t>
+  </si>
+  <si>
+    <t>Wage inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Real marginal cost</t>
+  </si>
+  <si>
+    <t>Measurement error on price inflation</t>
+  </si>
+  <si>
+    <t>Measurement error on wage inflation</t>
+  </si>
+  <si>
+    <t>Consumption demand shock</t>
+  </si>
+  <si>
+    <t>Cost push shock</t>
+  </si>
+  <si>
+    <t>Productivity shock</t>
+  </si>
+  <si>
+    <t>Policy shock</t>
+  </si>
+  <si>
+    <t>Long-term rate shock</t>
+  </si>
+  <si>
+    <t>Wage shock</t>
+  </si>
+  <si>
+    <t>Long run growth</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Labor share</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Fixed level of capital</t>
+  </si>
+  <si>
+    <t>Inflation target</t>
+  </si>
+  <si>
+    <t>Elasticity of substitution in monopoly markets</t>
+  </si>
+  <si>
+    <t>Inverse elasticity of labor supply</t>
+  </si>
+  <si>
+    <t>Habit</t>
+  </si>
+  <si>
+    <t>Wage stickiness</t>
+  </si>
+  <si>
+    <t>Price stickiness</t>
+  </si>
+  <si>
+    <t>Autoregression in productivity</t>
+  </si>
+  <si>
+    <t>Autoregression in short rate</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to inflation</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to labor</t>
+  </si>
+  <si>
+    <t>Autoregression in 5-year term premium</t>
+  </si>
+  <si>
+    <t>Intercept in short rate</t>
+  </si>
+  <si>
+    <t>Intercept in long rate</t>
+  </si>
+  <si>
+    <t>Intercept in inflation rate</t>
+  </si>
+  <si>
+    <t>Intercept in output growth rate</t>
+  </si>
+  <si>
+    <t>Intercept in wage inflation rate</t>
   </si>
   <si>
     <t>Time trend</t>
@@ -4548,7 +5610,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -4569,11 +5631,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -4588,6 +5653,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4609,24 +5677,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1387</v>
+        <v>1741</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1442</v>
+        <v>1796</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1443</v>
+        <v>1797</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1444</v>
+        <v>1798</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1450</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1388</v>
+        <v>1742</v>
       </c>
       <c r="B2" s="0">
         <v>7.1827411167511901</v>
@@ -4635,15 +5703,15 @@
         <v>0</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1445</v>
+        <v>1799</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>1451</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>1389</v>
+        <v>1743</v>
       </c>
       <c r="B3" s="0">
         <v>7.1827411167511901</v>
@@ -4652,15 +5720,15 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1445</v>
+        <v>1799</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1452</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1390</v>
+        <v>1744</v>
       </c>
       <c r="B4" s="0">
         <v>2.4999999999999467</v>
@@ -4669,15 +5737,15 @@
         <v>2.960594732333751e-14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1445</v>
+        <v>1799</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1453</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>1391</v>
+        <v>1745</v>
       </c>
       <c r="B5" s="0">
         <v>2.9999999999999583</v>
@@ -4686,15 +5754,15 @@
         <v>3.7007434154171883e-14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1445</v>
+        <v>1799</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1454</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>1392</v>
+        <v>1746</v>
       </c>
       <c r="B6" s="0">
         <v>5.5749999999999744</v>
@@ -4703,15 +5771,15 @@
         <v>0</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1445</v>
+        <v>1799</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1455</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>1393</v>
+        <v>1747</v>
       </c>
       <c r="B7" s="0">
         <v>1.5519465293293773</v>
@@ -4720,15 +5788,15 @@
         <v>1.0074170717777329</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1456</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>1394</v>
+        <v>1748</v>
       </c>
       <c r="B8" s="0">
         <v>0.74698177564761814</v>
@@ -4737,15 +5805,15 @@
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>1457</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>1395</v>
+        <v>1749</v>
       </c>
       <c r="B9" s="0">
         <v>1.7313525130113012</v>
@@ -4754,15 +5822,15 @@
         <v>1.0136552464388315</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1458</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>1396</v>
+        <v>1750</v>
       </c>
       <c r="B10" s="0">
         <v>0.83333333333333337</v>
@@ -4771,15 +5839,15 @@
         <v>1.0061922463256359</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>1459</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>1397</v>
+        <v>1751</v>
       </c>
       <c r="B11" s="0">
         <v>1.5519465293293773</v>
@@ -4788,15 +5856,15 @@
         <v>1.0074170717777329</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>1460</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>1398</v>
+        <v>1752</v>
       </c>
       <c r="B12" s="0">
         <v>1</v>
@@ -4805,15 +5873,15 @@
         <v>1.0074170717777329</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>1461</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>1399</v>
+        <v>1753</v>
       </c>
       <c r="B13" s="0">
         <v>1.0074170717777329</v>
@@ -4822,15 +5890,15 @@
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>1462</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>1400</v>
+        <v>1754</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
@@ -4839,15 +5907,15 @@
         <v>1.0061922463256359</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>1463</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>1401</v>
+        <v>1755</v>
       </c>
       <c r="B15" s="0">
         <v>1.0174924957880032</v>
@@ -4856,15 +5924,15 @@
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>1464</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>1402</v>
+        <v>1756</v>
       </c>
       <c r="B16" s="0">
         <v>1.0174924957880032</v>
@@ -4873,15 +5941,15 @@
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>1465</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>1403</v>
+        <v>1757</v>
       </c>
       <c r="B17" s="0">
         <v>1.0174924957880032</v>
@@ -4890,15 +5958,15 @@
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1446</v>
+        <v>1800</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>1466</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>1404</v>
+        <v>1758</v>
       </c>
       <c r="B18" s="0">
         <v>0</v>
@@ -4907,15 +5975,15 @@
         <v>0</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1447</v>
+        <v>1801</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>1467</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>1405</v>
+        <v>1759</v>
       </c>
       <c r="B19" s="0">
         <v>1.5311735582264343</v>
@@ -4924,15 +5992,15 @@
         <v>1.0136552464388342</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1468</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>1406</v>
+        <v>1760</v>
       </c>
       <c r="B20" s="0">
         <v>0.051731550977645917</v>
@@ -4941,15 +6009,15 @@
         <v>1.0136552464388313</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>1469</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>1407</v>
+        <v>1761</v>
       </c>
       <c r="B21" s="0">
         <v>0.64435209661000203</v>
@@ -4958,15 +6026,15 @@
         <v>0.98652870738172072</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>1470</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>1408</v>
+        <v>1762</v>
       </c>
       <c r="B22" s="0">
         <v>1.0061922463256359</v>
@@ -4975,15 +6043,15 @@
         <v>1</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>1471</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>1409</v>
+        <v>1763</v>
       </c>
       <c r="B23" s="0">
         <v>1.0249999999999995</v>
@@ -4992,15 +6060,15 @@
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1472</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>1410</v>
+        <v>1764</v>
       </c>
       <c r="B24" s="0">
         <v>1.0136552464388315</v>
@@ -5009,15 +6077,15 @@
         <v>1</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>1473</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>1411</v>
+        <v>1765</v>
       </c>
       <c r="B25" s="0">
         <v>0.83333333333333337</v>
@@ -5026,15 +6094,15 @@
         <v>1</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>1448</v>
+        <v>1802</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>1474</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>1412</v>
+        <v>1766</v>
       </c>
       <c r="B26" s="0">
         <v>0</v>
@@ -5042,16 +6110,14 @@
       <c r="C26" s="0">
         <v>0</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D26" s="0"/>
       <c r="E26" s="0" t="s">
-        <v>1475</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>1413</v>
+        <v>1767</v>
       </c>
       <c r="B27" s="0">
         <v>0</v>
@@ -5059,16 +6125,14 @@
       <c r="C27" s="0">
         <v>0</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D27" s="0"/>
       <c r="E27" s="0" t="s">
-        <v>1476</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>1414</v>
+        <v>1768</v>
       </c>
       <c r="B28" s="0">
         <v>0</v>
@@ -5076,16 +6140,14 @@
       <c r="C28" s="0">
         <v>0</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D28" s="0"/>
       <c r="E28" s="0" t="s">
-        <v>1477</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>1415</v>
+        <v>1769</v>
       </c>
       <c r="B29" s="0">
         <v>0</v>
@@ -5093,16 +6155,14 @@
       <c r="C29" s="0">
         <v>0</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D29" s="0"/>
       <c r="E29" s="0" t="s">
-        <v>1478</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>1416</v>
+        <v>1770</v>
       </c>
       <c r="B30" s="0">
         <v>0</v>
@@ -5110,16 +6170,14 @@
       <c r="C30" s="0">
         <v>0</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D30" s="0"/>
       <c r="E30" s="0" t="s">
-        <v>1479</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>1417</v>
+        <v>1771</v>
       </c>
       <c r="B31" s="0">
         <v>0</v>
@@ -5127,16 +6185,14 @@
       <c r="C31" s="0">
         <v>0</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D31" s="0"/>
       <c r="E31" s="0" t="s">
-        <v>1480</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>1418</v>
+        <v>1772</v>
       </c>
       <c r="B32" s="0">
         <v>0</v>
@@ -5144,16 +6200,14 @@
       <c r="C32" s="0">
         <v>0</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D32" s="0"/>
       <c r="E32" s="0" t="s">
-        <v>1481</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>1419</v>
+        <v>1773</v>
       </c>
       <c r="B33" s="0">
         <v>0</v>
@@ -5161,16 +6215,14 @@
       <c r="C33" s="0">
         <v>0</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D33" s="0"/>
       <c r="E33" s="0" t="s">
-        <v>1482</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>1420</v>
+        <v>1774</v>
       </c>
       <c r="B34" s="0">
         <v>1.0074170717777329</v>
@@ -5178,16 +6230,14 @@
       <c r="C34" s="0">
         <v>0</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D34" s="0"/>
       <c r="E34" s="0" t="s">
-        <v>1483</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>1421</v>
+        <v>1775</v>
       </c>
       <c r="B35" s="0">
         <v>0.99622871975463567</v>
@@ -5195,16 +6245,14 @@
       <c r="C35" s="0">
         <v>0</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D35" s="0"/>
       <c r="E35" s="0" t="s">
-        <v>1484</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>1422</v>
+        <v>1776</v>
       </c>
       <c r="B36" s="0">
         <v>0.59999999999999998</v>
@@ -5212,16 +6260,14 @@
       <c r="C36" s="0">
         <v>0</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D36" s="0"/>
       <c r="E36" s="0" t="s">
-        <v>1485</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>1423</v>
+        <v>1777</v>
       </c>
       <c r="B37" s="0">
         <v>0.029999999999999999</v>
@@ -5229,16 +6275,14 @@
       <c r="C37" s="0">
         <v>0</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D37" s="0"/>
       <c r="E37" s="0" t="s">
-        <v>1486</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>1424</v>
+        <v>1778</v>
       </c>
       <c r="B38" s="0">
         <v>10</v>
@@ -5246,16 +6290,14 @@
       <c r="C38" s="0">
         <v>0</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D38" s="0"/>
       <c r="E38" s="0" t="s">
-        <v>1487</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>1425</v>
+        <v>1779</v>
       </c>
       <c r="B39" s="0">
         <v>1.0061922463256359</v>
@@ -5263,16 +6305,14 @@
       <c r="C39" s="0">
         <v>0</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D39" s="0"/>
       <c r="E39" s="0" t="s">
-        <v>1488</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>1426</v>
+        <v>1780</v>
       </c>
       <c r="B40" s="0">
         <v>6</v>
@@ -5280,16 +6320,14 @@
       <c r="C40" s="0">
         <v>0</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D40" s="0"/>
       <c r="E40" s="0" t="s">
-        <v>1489</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>1427</v>
+        <v>1781</v>
       </c>
       <c r="B41" s="0">
         <v>0.25</v>
@@ -5297,16 +6335,14 @@
       <c r="C41" s="0">
         <v>0</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D41" s="0"/>
       <c r="E41" s="0" t="s">
-        <v>1490</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>1428</v>
+        <v>1782</v>
       </c>
       <c r="B42" s="0">
         <v>0.84999999999999998</v>
@@ -5314,16 +6350,14 @@
       <c r="C42" s="0">
         <v>0</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D42" s="0"/>
       <c r="E42" s="0" t="s">
-        <v>1491</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>1429</v>
+        <v>1783</v>
       </c>
       <c r="B43" s="0">
         <v>60</v>
@@ -5331,16 +6365,14 @@
       <c r="C43" s="0">
         <v>0</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D43" s="0"/>
       <c r="E43" s="0" t="s">
-        <v>1492</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>1430</v>
+        <v>1784</v>
       </c>
       <c r="B44" s="0">
         <v>300</v>
@@ -5348,16 +6380,14 @@
       <c r="C44" s="0">
         <v>0</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D44" s="0"/>
       <c r="E44" s="0" t="s">
-        <v>1493</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>1431</v>
+        <v>1785</v>
       </c>
       <c r="B45" s="0">
         <v>0.90000000000000002</v>
@@ -5365,16 +6395,14 @@
       <c r="C45" s="0">
         <v>0</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D45" s="0"/>
       <c r="E45" s="0" t="s">
-        <v>1494</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>1432</v>
+        <v>1786</v>
       </c>
       <c r="B46" s="0">
         <v>0.84999999999999998</v>
@@ -5382,16 +6410,14 @@
       <c r="C46" s="0">
         <v>0</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D46" s="0"/>
       <c r="E46" s="0" t="s">
-        <v>1495</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>1433</v>
+        <v>1787</v>
       </c>
       <c r="B47" s="0">
         <v>3.5</v>
@@ -5399,16 +6425,14 @@
       <c r="C47" s="0">
         <v>0</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D47" s="0"/>
       <c r="E47" s="0" t="s">
-        <v>1496</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>1434</v>
+        <v>1788</v>
       </c>
       <c r="B48" s="0">
         <v>0</v>
@@ -5416,16 +6440,14 @@
       <c r="C48" s="0">
         <v>0</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D48" s="0"/>
       <c r="E48" s="0" t="s">
-        <v>1497</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>1435</v>
+        <v>1789</v>
       </c>
       <c r="B49" s="0">
         <v>0.80000000000000004</v>
@@ -5433,16 +6455,14 @@
       <c r="C49" s="0">
         <v>0</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D49" s="0"/>
       <c r="E49" s="0" t="s">
-        <v>1498</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>1436</v>
+        <v>1790</v>
       </c>
       <c r="B50" s="0">
         <v>0</v>
@@ -5450,16 +6470,14 @@
       <c r="C50" s="0">
         <v>0</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D50" s="0"/>
       <c r="E50" s="0" t="s">
-        <v>1499</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>1437</v>
+        <v>1791</v>
       </c>
       <c r="B51" s="0">
         <v>0</v>
@@ -5467,16 +6485,14 @@
       <c r="C51" s="0">
         <v>0</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D51" s="0"/>
       <c r="E51" s="0" t="s">
-        <v>1500</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>1438</v>
+        <v>1792</v>
       </c>
       <c r="B52" s="0">
         <v>0</v>
@@ -5484,16 +6500,14 @@
       <c r="C52" s="0">
         <v>0</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D52" s="0"/>
       <c r="E52" s="0" t="s">
-        <v>1501</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>1439</v>
+        <v>1793</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
@@ -5501,16 +6515,14 @@
       <c r="C53" s="0">
         <v>0</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D53" s="0"/>
       <c r="E53" s="0" t="s">
-        <v>1502</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>1440</v>
+        <v>1794</v>
       </c>
       <c r="B54" s="0">
         <v>0</v>
@@ -5518,16 +6530,14 @@
       <c r="C54" s="0">
         <v>0</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>1449</v>
-      </c>
+      <c r="D54" s="0"/>
       <c r="E54" s="0" t="s">
-        <v>1503</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>1441</v>
+        <v>1795</v>
       </c>
       <c r="B55" s="0">
         <v>0</v>
@@ -5536,10 +6546,10 @@
         <v>1</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>1449</v>
+        <v>1803</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>1504</v>
+        <v>1858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgraded filter to kalmanFilter
</commit_message>
<xml_diff>
--- a/steady.xlsx
+++ b/steady.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5601" uniqueCount="4417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5747" uniqueCount="4542">
   <si>
     <t>Row</t>
   </si>
@@ -10003,6 +10003,381 @@
   </si>
   <si>
     <t>beta0</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>xiw</t>
+  </si>
+  <si>
+    <t>xip</t>
+  </si>
+  <si>
+    <t>rhoa</t>
+  </si>
+  <si>
+    <t>rhor</t>
+  </si>
+  <si>
+    <t>kappap</t>
+  </si>
+  <si>
+    <t>kappan</t>
+  </si>
+  <si>
+    <t>rhoterm20</t>
+  </si>
+  <si>
+    <t>Short_</t>
+  </si>
+  <si>
+    <t>Long_</t>
+  </si>
+  <si>
+    <t>Infl_</t>
+  </si>
+  <si>
+    <t>Growth_</t>
+  </si>
+  <si>
+    <t>Wage_</t>
+  </si>
+  <si>
+    <t>ttrend</t>
+  </si>
+  <si>
+    <t>SteadyLevel_1</t>
+  </si>
+  <si>
+    <t>SteadyLevel_2</t>
+  </si>
+  <si>
+    <t>SteadyChange_1</t>
+  </si>
+  <si>
+    <t>SteadyChange_2</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Rate/</t>
+  </si>
+  <si>
+    <t>Diff–</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Short term rate</t>
+  </si>
+  <si>
+    <t>Long term rate</t>
+  </si>
+  <si>
+    <t>Price inflation</t>
+  </si>
+  <si>
+    <t>Output growth</t>
+  </si>
+  <si>
+    <t>Wage inflation</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Wage rate</t>
+  </si>
+  <si>
+    <t>Nominal marginal cost</t>
+  </si>
+  <si>
+    <t>Consumption habit</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Rate of change in productivity</t>
+  </si>
+  <si>
+    <t>Final prices</t>
+  </si>
+  <si>
+    <t>Nominal interest rate</t>
+  </si>
+  <si>
+    <t>Real interest rate</t>
+  </si>
+  <si>
+    <t>5-year interest rate</t>
+  </si>
+  <si>
+    <t>5-Year expectations of short rates</t>
+  </si>
+  <si>
+    <t>5-year term premium</t>
+  </si>
+  <si>
+    <t>Price of capital</t>
+  </si>
+  <si>
+    <t>Rental price of capital</t>
+  </si>
+  <si>
+    <t>Households shadow value of wealth</t>
+  </si>
+  <si>
+    <t>Inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Inflation Y/Y</t>
+  </si>
+  <si>
+    <t>Wage inflation Q/Q</t>
+  </si>
+  <si>
+    <t>Real marginal cost</t>
+  </si>
+  <si>
+    <t>Measurement error on price inflation</t>
+  </si>
+  <si>
+    <t>Measurement error on wage inflation</t>
+  </si>
+  <si>
+    <t>Consumption demand shock</t>
+  </si>
+  <si>
+    <t>Cost push shock</t>
+  </si>
+  <si>
+    <t>Productivity shock</t>
+  </si>
+  <si>
+    <t>Policy shock</t>
+  </si>
+  <si>
+    <t>Long-term rate shock</t>
+  </si>
+  <si>
+    <t>Wage shock</t>
+  </si>
+  <si>
+    <t>Long run growth</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Utility of net worth parameter</t>
+  </si>
+  <si>
+    <t>Labor share</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Fixed level of capital</t>
+  </si>
+  <si>
+    <t>Inflation target</t>
+  </si>
+  <si>
+    <t>Elasticity of substitution in monopoly markets</t>
+  </si>
+  <si>
+    <t>Inverse elasticity of labor supply</t>
+  </si>
+  <si>
+    <t>Habit</t>
+  </si>
+  <si>
+    <t>Wage stickiness</t>
+  </si>
+  <si>
+    <t>Price stickiness</t>
+  </si>
+  <si>
+    <t>Autoregression in productivity</t>
+  </si>
+  <si>
+    <t>Autoregression in short rate</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to inflation</t>
+  </si>
+  <si>
+    <t>Monetary policy reaction to labor</t>
+  </si>
+  <si>
+    <t>Autoregression in 5-year term premium</t>
+  </si>
+  <si>
+    <t>Intercept in short rate</t>
+  </si>
+  <si>
+    <t>Intercept in long rate</t>
+  </si>
+  <si>
+    <t>Intercept in inflation rate</t>
+  </si>
+  <si>
+    <t>Intercept in output growth rate</t>
+  </si>
+  <si>
+    <t>Intercept in wage inflation rate</t>
+  </si>
+  <si>
+    <t>Time trend</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Infl</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Wage</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>dA</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R20exp</t>
+  </si>
+  <si>
+    <t>term20</t>
+  </si>
+  <si>
+    <t>Pk</t>
+  </si>
+  <si>
+    <t>Rk</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>dP</t>
+  </si>
+  <si>
+    <t>d4P</t>
+  </si>
+  <si>
+    <t>dW</t>
+  </si>
+  <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>Mp</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>Ey</t>
+  </si>
+  <si>
+    <t>Ep</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t>Er</t>
+  </si>
+  <si>
+    <t>Eterm20</t>
+  </si>
+  <si>
+    <t>Ew</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>beta0</t>
+  </si>
+  <si>
+    <t>beta1</t>
   </si>
   <si>
     <t>gamma</t>
@@ -13353,30 +13728,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>4292</v>
+        <v>4417</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4350</v>
+        <v>4475</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4351</v>
+        <v>4476</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>4352</v>
+        <v>4477</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4353</v>
+        <v>4478</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>4354</v>
+        <v>4479</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>4360</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>4293</v>
+        <v>4418</v>
       </c>
       <c r="B2" s="0">
         <v>3.0199999999999783</v>
@@ -13391,15 +13766,15 @@
         <v>-6.0623640334538528e-17</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>4355</v>
+        <v>4480</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>4361</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>4294</v>
+        <v>4419</v>
       </c>
       <c r="B3" s="0">
         <v>3.0199999999999783</v>
@@ -13414,15 +13789,15 @@
         <v>4.7968950373470761e-17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>4355</v>
+        <v>4480</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>4362</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>4295</v>
+        <v>4420</v>
       </c>
       <c r="B4" s="0">
         <v>2.000000000000024</v>
@@ -13437,15 +13812,15 @@
         <v>-3.0174676778304199e-17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>4355</v>
+        <v>4480</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>4363</v>
+        <v>4488</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4296</v>
+        <v>4421</v>
       </c>
       <c r="B5" s="0">
         <v>2.4999999999998579</v>
@@ -13460,15 +13835,15 @@
         <v>1.7537675456253333e-14</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>4355</v>
+        <v>4480</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>4364</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>4297</v>
+        <v>4422</v>
       </c>
       <c r="B6" s="0">
         <v>4.5499999999999652</v>
@@ -13483,15 +13858,15 @@
         <v>1.7342571379942422e-14</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>4355</v>
+        <v>4480</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>4365</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>4298</v>
+        <v>4423</v>
       </c>
       <c r="B7" s="0">
         <v>1.5519465293293777</v>
@@ -13506,15 +13881,15 @@
         <v>1.0049629315732038</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>4366</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>4299</v>
+        <v>4424</v>
       </c>
       <c r="B8" s="0">
         <v>0.74698177564761814</v>
@@ -13529,15 +13904,15 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>4367</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>4300</v>
+        <v>4425</v>
       </c>
       <c r="B9" s="0">
         <v>1.7313525130113014</v>
@@ -13552,15 +13927,15 @@
         <v>1.0099504938362081</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>4368</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>4301</v>
+        <v>4426</v>
       </c>
       <c r="B10" s="0">
         <v>0.83333333333333337</v>
@@ -13575,15 +13950,15 @@
         <v>1.0049629315732036</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>4369</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>4302</v>
+        <v>4427</v>
       </c>
       <c r="B11" s="0">
         <v>1.5519465293293777</v>
@@ -13598,15 +13973,15 @@
         <v>1.0049629315732038</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>4370</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>4303</v>
+        <v>4428</v>
       </c>
       <c r="B12" s="0">
         <v>1</v>
@@ -13621,15 +13996,15 @@
         <v>1.0049629315732038</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>4371</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>4304</v>
+        <v>4429</v>
       </c>
       <c r="B13" s="0">
         <v>1.0061922463256359</v>
@@ -13644,15 +14019,15 @@
         <v>1</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>4372</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>4305</v>
+        <v>4430</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
@@ -13667,15 +14042,15 @@
         <v>1.0049629315732038</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>4373</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>4306</v>
+        <v>4431</v>
       </c>
       <c r="B15" s="0">
         <v>1.0074659719585326</v>
@@ -13690,15 +14065,15 @@
         <v>1</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>4374</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>4307</v>
+        <v>4432</v>
       </c>
       <c r="B16" s="0">
         <v>1.0024906793143211</v>
@@ -13713,15 +14088,15 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>4375</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>4308</v>
+        <v>4433</v>
       </c>
       <c r="B17" s="0">
         <v>1.0074659719585326</v>
@@ -13736,15 +14111,15 @@
         <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>4376</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>4309</v>
+        <v>4434</v>
       </c>
       <c r="B18" s="0">
         <v>1.0074659719585326</v>
@@ -13759,15 +14134,15 @@
         <v>1</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>4356</v>
+        <v>4481</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>4377</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>4310</v>
+        <v>4435</v>
       </c>
       <c r="B19" s="0">
         <v>0</v>
@@ -13782,15 +14157,15 @@
         <v>-1.4899097114009449e-24</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>4357</v>
+        <v>4482</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>4378</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>4311</v>
+        <v>4436</v>
       </c>
       <c r="B20" s="0">
         <v>1.5311735582263752</v>
@@ -13805,15 +14180,15 @@
         <v>1.0099504938362083</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>4379</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>4312</v>
+        <v>4437</v>
       </c>
       <c r="B21" s="0">
         <v>0.051731550977645938</v>
@@ -13828,15 +14203,15 @@
         <v>1.0099504938362078</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>4380</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>4313</v>
+        <v>4438</v>
       </c>
       <c r="B22" s="0">
         <v>0.64435209661000181</v>
@@ -13851,15 +14226,15 @@
         <v>0.99014754297667418</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>4381</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>4314</v>
+        <v>4439</v>
       </c>
       <c r="B23" s="0">
         <v>1.0049629315732038</v>
@@ -13874,15 +14249,15 @@
         <v>1</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>4382</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>4315</v>
+        <v>4440</v>
       </c>
       <c r="B24" s="0">
         <v>1.0200000000000002</v>
@@ -13897,15 +14272,15 @@
         <v>1.0000000000000002</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>4383</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>4316</v>
+        <v>4441</v>
       </c>
       <c r="B25" s="0">
         <v>1.0111859095936382</v>
@@ -13920,15 +14295,15 @@
         <v>1</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>4384</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>4317</v>
+        <v>4442</v>
       </c>
       <c r="B26" s="0">
         <v>0.83333333333333337</v>
@@ -13943,15 +14318,15 @@
         <v>1</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>4358</v>
+        <v>4483</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>4385</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>4318</v>
+        <v>4443</v>
       </c>
       <c r="B27" s="0">
         <v>0</v>
@@ -13967,12 +14342,12 @@
       </c>
       <c r="F27" s="0"/>
       <c r="G27" s="0" t="s">
-        <v>4386</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>4319</v>
+        <v>4444</v>
       </c>
       <c r="B28" s="0">
         <v>0</v>
@@ -13988,12 +14363,12 @@
       </c>
       <c r="F28" s="0"/>
       <c r="G28" s="0" t="s">
-        <v>4387</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>4320</v>
+        <v>4445</v>
       </c>
       <c r="B29" s="0">
         <v>0</v>
@@ -14009,12 +14384,12 @@
       </c>
       <c r="F29" s="0"/>
       <c r="G29" s="0" t="s">
-        <v>4388</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>4321</v>
+        <v>4446</v>
       </c>
       <c r="B30" s="0">
         <v>0</v>
@@ -14030,12 +14405,12 @@
       </c>
       <c r="F30" s="0"/>
       <c r="G30" s="0" t="s">
-        <v>4389</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>4322</v>
+        <v>4447</v>
       </c>
       <c r="B31" s="0">
         <v>0</v>
@@ -14051,12 +14426,12 @@
       </c>
       <c r="F31" s="0"/>
       <c r="G31" s="0" t="s">
-        <v>4390</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>4323</v>
+        <v>4448</v>
       </c>
       <c r="B32" s="0">
         <v>0</v>
@@ -14072,12 +14447,12 @@
       </c>
       <c r="F32" s="0"/>
       <c r="G32" s="0" t="s">
-        <v>4391</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>4324</v>
+        <v>4449</v>
       </c>
       <c r="B33" s="0">
         <v>0</v>
@@ -14093,12 +14468,12 @@
       </c>
       <c r="F33" s="0"/>
       <c r="G33" s="0" t="s">
-        <v>4392</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>4325</v>
+        <v>4450</v>
       </c>
       <c r="B34" s="0">
         <v>0</v>
@@ -14114,12 +14489,12 @@
       </c>
       <c r="F34" s="0"/>
       <c r="G34" s="0" t="s">
-        <v>4393</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>4326</v>
+        <v>4451</v>
       </c>
       <c r="B35" s="0">
         <v>1.0061922463256359</v>
@@ -14135,12 +14510,12 @@
       </c>
       <c r="F35" s="0"/>
       <c r="G35" s="0" t="s">
-        <v>4394</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>4327</v>
+        <v>4452</v>
       </c>
       <c r="B36" s="0">
         <v>0.99622871975463567</v>
@@ -14156,12 +14531,12 @@
       </c>
       <c r="F36" s="0"/>
       <c r="G36" s="0" t="s">
-        <v>4395</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>4328</v>
+        <v>4453</v>
       </c>
       <c r="B37" s="0">
         <v>-0.0074361935641006766</v>
@@ -14177,12 +14552,12 @@
       </c>
       <c r="F37" s="0"/>
       <c r="G37" s="0" t="s">
-        <v>4396</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>4329</v>
+        <v>4454</v>
       </c>
       <c r="B38" s="0">
         <v>0.80000000000000004</v>
@@ -14201,7 +14576,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>4330</v>
+        <v>4455</v>
       </c>
       <c r="B39" s="0">
         <v>0.59999999999999998</v>
@@ -14217,12 +14592,12 @@
       </c>
       <c r="F39" s="0"/>
       <c r="G39" s="0" t="s">
-        <v>4397</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>4331</v>
+        <v>4456</v>
       </c>
       <c r="B40" s="0">
         <v>0.029999999999999999</v>
@@ -14238,12 +14613,12 @@
       </c>
       <c r="F40" s="0"/>
       <c r="G40" s="0" t="s">
-        <v>4398</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>4332</v>
+        <v>4457</v>
       </c>
       <c r="B41" s="0">
         <v>10</v>
@@ -14259,12 +14634,12 @@
       </c>
       <c r="F41" s="0"/>
       <c r="G41" s="0" t="s">
-        <v>4399</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>4333</v>
+        <v>4458</v>
       </c>
       <c r="B42" s="0">
         <v>1.0049629315732038</v>
@@ -14280,12 +14655,12 @@
       </c>
       <c r="F42" s="0"/>
       <c r="G42" s="0" t="s">
-        <v>4400</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>4334</v>
+        <v>4459</v>
       </c>
       <c r="B43" s="0">
         <v>6</v>
@@ -14301,12 +14676,12 @@
       </c>
       <c r="F43" s="0"/>
       <c r="G43" s="0" t="s">
-        <v>4401</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>4335</v>
+        <v>4460</v>
       </c>
       <c r="B44" s="0">
         <v>0.25</v>
@@ -14322,12 +14697,12 @@
       </c>
       <c r="F44" s="0"/>
       <c r="G44" s="0" t="s">
-        <v>4402</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>4336</v>
+        <v>4461</v>
       </c>
       <c r="B45" s="0">
         <v>0.84999999999999998</v>
@@ -14343,12 +14718,12 @@
       </c>
       <c r="F45" s="0"/>
       <c r="G45" s="0" t="s">
-        <v>4403</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>4337</v>
+        <v>4462</v>
       </c>
       <c r="B46" s="0">
         <v>60</v>
@@ -14364,12 +14739,12 @@
       </c>
       <c r="F46" s="0"/>
       <c r="G46" s="0" t="s">
-        <v>4404</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>4338</v>
+        <v>4463</v>
       </c>
       <c r="B47" s="0">
         <v>300</v>
@@ -14385,12 +14760,12 @@
       </c>
       <c r="F47" s="0"/>
       <c r="G47" s="0" t="s">
-        <v>4405</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>4339</v>
+        <v>4464</v>
       </c>
       <c r="B48" s="0">
         <v>0.90000000000000002</v>
@@ -14406,12 +14781,12 @@
       </c>
       <c r="F48" s="0"/>
       <c r="G48" s="0" t="s">
-        <v>4406</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>4340</v>
+        <v>4465</v>
       </c>
       <c r="B49" s="0">
         <v>0.84999999999999998</v>
@@ -14427,12 +14802,12 @@
       </c>
       <c r="F49" s="0"/>
       <c r="G49" s="0" t="s">
-        <v>4407</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>4341</v>
+        <v>4466</v>
       </c>
       <c r="B50" s="0">
         <v>4</v>
@@ -14448,12 +14823,12 @@
       </c>
       <c r="F50" s="0"/>
       <c r="G50" s="0" t="s">
-        <v>4408</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>4342</v>
+        <v>4467</v>
       </c>
       <c r="B51" s="0">
         <v>0</v>
@@ -14469,12 +14844,12 @@
       </c>
       <c r="F51" s="0"/>
       <c r="G51" s="0" t="s">
-        <v>4409</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>4343</v>
+        <v>4468</v>
       </c>
       <c r="B52" s="0">
         <v>0.80000000000000004</v>
@@ -14490,12 +14865,12 @@
       </c>
       <c r="F52" s="0"/>
       <c r="G52" s="0" t="s">
-        <v>4410</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>4344</v>
+        <v>4469</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
@@ -14511,12 +14886,12 @@
       </c>
       <c r="F53" s="0"/>
       <c r="G53" s="0" t="s">
-        <v>4411</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>4345</v>
+        <v>4470</v>
       </c>
       <c r="B54" s="0">
         <v>0</v>
@@ -14532,12 +14907,12 @@
       </c>
       <c r="F54" s="0"/>
       <c r="G54" s="0" t="s">
-        <v>4412</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>4346</v>
+        <v>4471</v>
       </c>
       <c r="B55" s="0">
         <v>0</v>
@@ -14553,12 +14928,12 @@
       </c>
       <c r="F55" s="0"/>
       <c r="G55" s="0" t="s">
-        <v>4413</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>4347</v>
+        <v>4472</v>
       </c>
       <c r="B56" s="0">
         <v>0</v>
@@ -14574,12 +14949,12 @@
       </c>
       <c r="F56" s="0"/>
       <c r="G56" s="0" t="s">
-        <v>4414</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>4348</v>
+        <v>4473</v>
       </c>
       <c r="B57" s="0">
         <v>0</v>
@@ -14595,12 +14970,12 @@
       </c>
       <c r="F57" s="0"/>
       <c r="G57" s="0" t="s">
-        <v>4415</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>4349</v>
+        <v>4474</v>
       </c>
       <c r="B58" s="0">
         <v>0</v>
@@ -14615,10 +14990,10 @@
         <v>1</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>4359</v>
+        <v>4484</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>4416</v>
+        <v>4541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>